<commit_message>
AlertIf + Unit-Test coverage
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D5EBD9-8E46-654A-9718-5F8391D6E0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC2862B-0F38-5843-A298-BC0D2BAAA41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16640" yWindow="3200" windowWidth="16720" windowHeight="17120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16640" yWindow="3200" windowWidth="16720" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
   <si>
     <t>Activity</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Baangt is the real deal!</t>
+  </si>
+  <si>
+    <t>alertif</t>
   </si>
 </sst>
 </file>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -870,18 +873,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -889,49 +886,46 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -943,86 +937,89 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1030,11 +1027,8 @@
       <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1042,27 +1036,27 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1070,134 +1064,137 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
       </c>
       <c r="C36" t="s">
         <v>79</v>
       </c>
-      <c r="E36" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" t="s">
-        <v>83</v>
+      <c r="D36" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" t="s">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1208,7 +1205,7 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1219,26 +1216,26 @@
         <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1249,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1260,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1271,24 +1268,35 @@
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1301,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
"Stage" added to data-tab
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A9DE66-1F2F-4C41-AF24-B7AFF46A9937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB0409-A2E8-6B4D-8A9F-771741D46AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="3200" windowWidth="27300" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
   <si>
     <t>Activity</t>
   </si>
@@ -752,7 +752,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1362,106 +1362,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>77</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>91</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{5CD7A5C0-5F13-8349-95E1-06370B6D7538}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{78541470-6199-8A4C-990C-13504A3484C0}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{5CD7A5C0-5F13-8349-95E1-06370B6D7538}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{78541470-6199-8A4C-990C-13504A3484C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Statistics and Logs update in gui
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/tests/0TestInput/ServiceTestInput/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79419D7D-7A44-E644-AC59-63FE95F88E6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16640" yWindow="3200" windowWidth="16720" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="3195" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="CustomerData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="114">
   <si>
     <t>Activity</t>
   </si>
@@ -116,9 +111,6 @@
     <t>//*[@id='lastName']</t>
   </si>
   <si>
-    <t>$(lastName1)</t>
-  </si>
-  <si>
     <t>//select[@id='country']</t>
   </si>
   <si>
@@ -143,18 +135,6 @@
     <t>//a[contains(., 'Download source code')]</t>
   </si>
   <si>
-    <t>firstName1</t>
-  </si>
-  <si>
-    <t>First form</t>
-  </si>
-  <si>
-    <t>lastName1</t>
-  </si>
-  <si>
-    <t>filled out</t>
-  </si>
-  <si>
     <t>textarea1</t>
   </si>
   <si>
@@ -182,12 +162,6 @@
     <t>this is an input</t>
   </si>
   <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Testcase</t>
-  </si>
-  <si>
     <t>Wonderful baangt!</t>
   </si>
   <si>
@@ -197,122 +171,200 @@
     <t>Country</t>
   </si>
   <si>
-    <t>England</t>
+    <t>clickif</t>
+  </si>
+  <si>
+    <t>//option[@value='$(Country)']</t>
+  </si>
+  <si>
+    <t>$(Country)</t>
+  </si>
+  <si>
+    <t>//textarea[@name='message']</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Baangt is great!</t>
+  </si>
+  <si>
+    <t>Baangt is fantastic!</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>doIframe</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>$(doIframe)</t>
+  </si>
+  <si>
+    <t>endif</t>
+  </si>
+  <si>
+    <t>handleiframe</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>goback</t>
+  </si>
+  <si>
+    <t>//div[@class='container mt-3']//div[1]//div[1]//div[1]//iframe[1]</t>
+  </si>
+  <si>
+    <t>//div[@class='row mt-3']//div[2]//div[1]//div[1]//iframe[1]</t>
+  </si>
+  <si>
+    <t>//a[contains(.,'iFrame')]</t>
+  </si>
+  <si>
+    <t>saveto</t>
+  </si>
+  <si>
+    <t>//div[contains(@id,'results')]</t>
+  </si>
+  <si>
+    <t>formResult</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>!=</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>$(FAKER.name)</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>ibanGenerated</t>
+  </si>
+  <si>
+    <t>$(ibanGenerated)</t>
+  </si>
+  <si>
+    <t>This is perfect!</t>
+  </si>
+  <si>
+    <t>Another input, how cool!</t>
+  </si>
+  <si>
+    <t>Baangt is the real deal!</t>
+  </si>
+  <si>
+    <t>alertif</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>NameFirst</t>
+  </si>
+  <si>
+    <t>NameLast</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Franzi</t>
+  </si>
+  <si>
+    <t>Meier</t>
+  </si>
+  <si>
+    <t>Rudolf</t>
+  </si>
+  <si>
+    <t>Huber</t>
+  </si>
+  <si>
+    <t>Nudl</t>
+  </si>
+  <si>
+    <t>Auk</t>
+  </si>
+  <si>
+    <t>PQA</t>
+  </si>
+  <si>
+    <t>Franz</t>
+  </si>
+  <si>
+    <t>Fritz</t>
+  </si>
+  <si>
+    <t>FQA</t>
+  </si>
+  <si>
+    <t>Friedrich</t>
+  </si>
+  <si>
+    <t>Nette</t>
+  </si>
+  <si>
+    <t>Susi</t>
+  </si>
+  <si>
+    <t>Böhzer</t>
+  </si>
+  <si>
+    <t>Onkel</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Hochreiter</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Albers</t>
+  </si>
+  <si>
+    <t>RemoteReadExample</t>
+  </si>
+  <si>
+    <t>$(NameLast)</t>
+  </si>
+  <si>
+    <t>RRD_[CustomerData,*,[Stage:[$(Stage)],Country:[$(Country)],IsActive:[X]]]</t>
   </si>
   <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>clickif</t>
-  </si>
-  <si>
-    <t>//option[@value='$(Country)']</t>
-  </si>
-  <si>
-    <t>$(Country)</t>
-  </si>
-  <si>
-    <t>//textarea[@name='message']</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Baangt is great!</t>
-  </si>
-  <si>
-    <t>Baangt is fantastic!</t>
-  </si>
-  <si>
-    <t>submit</t>
-  </si>
-  <si>
-    <t>doIframe</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>$(doIframe)</t>
-  </si>
-  <si>
-    <t>endif</t>
-  </si>
-  <si>
-    <t>handleiframe</t>
-  </si>
-  <si>
-    <t>pause</t>
-  </si>
-  <si>
-    <t>goback</t>
-  </si>
-  <si>
-    <t>//div[@class='container mt-3']//div[1]//div[1]//div[1]//iframe[1]</t>
-  </si>
-  <si>
-    <t>//div[@class='row mt-3']//div[2]//div[1]//div[1]//iframe[1]</t>
-  </si>
-  <si>
-    <t>//a[contains(.,'iFrame')]</t>
-  </si>
-  <si>
-    <t>saveto</t>
-  </si>
-  <si>
-    <t>//div[contains(@id,'results')]</t>
-  </si>
-  <si>
-    <t>formResult</t>
-  </si>
-  <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>!=</t>
-  </si>
-  <si>
-    <t>""</t>
-  </si>
-  <si>
-    <t>$(FAKER.name)</t>
-  </si>
-  <si>
-    <t>IBAN</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>ibanGenerated</t>
-  </si>
-  <si>
-    <t>$(ibanGenerated)</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>This is perfect!</t>
-  </si>
-  <si>
-    <t>Another input, how cool!</t>
-  </si>
-  <si>
-    <t>Baangt is the real deal!</t>
-  </si>
-  <si>
-    <t>alertif</t>
+    <t>USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +378,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -352,13 +410,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,7 +433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,7 +475,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,27 +507,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,24 +541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -693,27 +716,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -753,7 +776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -764,18 +787,18 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -786,7 +809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -797,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -808,7 +831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -819,7 +842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -830,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -841,7 +864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -852,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -863,20 +886,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -887,7 +910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -901,7 +924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -912,7 +935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -923,7 +946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -931,13 +954,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -945,13 +968,13 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -962,7 +985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -973,7 +996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -984,7 +1007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -995,7 +1018,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1006,7 +1029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1039,10 +1062,10 @@
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1053,38 +1076,38 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
       <c r="D30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1092,21 +1115,21 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1114,52 +1137,52 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1170,15 +1193,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1186,18 +1209,18 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1205,73 +1228,73 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1282,22 +1305,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1306,120 +1329,301 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{5CD7A5C0-5F13-8349-95E1-06370B6D7538}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{78541470-6199-8A4C-990C-13504A3484C0}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proper handling of STAGE with data files (=ignore if datarecord stage <> stage from globals)
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B440BB-570F-BE43-A27A-4162B63B84B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="3195" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="6060" yWindow="3200" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="114">
   <si>
     <t>Activity</t>
   </si>
@@ -363,8 +369,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,8 +422,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,7 +439,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -475,7 +481,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,9 +513,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,6 +565,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -716,27 +758,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -776,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -790,7 +832,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -798,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -809,7 +851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -820,7 +862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -831,7 +873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -842,7 +884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -853,7 +895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -864,7 +906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -875,7 +917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -886,12 +928,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -899,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -910,7 +952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -924,7 +966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -935,7 +977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -946,7 +988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -960,7 +1002,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -974,7 +1016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -985,7 +1027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -996,7 +1038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1007,7 +1049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1018,7 +1060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1029,7 +1071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1040,7 +1082,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1065,7 +1107,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1079,7 +1121,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1093,7 +1135,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1107,7 +1149,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1160,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1129,7 +1171,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1143,7 +1185,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1154,7 +1196,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -1168,7 +1210,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1182,7 +1224,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -1201,7 +1243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1212,7 +1254,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -1220,7 +1262,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1273,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1284,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1295,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -1261,7 +1303,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +1314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -1294,7 +1336,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1305,7 +1347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1313,12 +1355,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1329,23 +1371,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1371,7 +1413,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1394,7 +1436,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1414,7 +1456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1437,28 +1479,166 @@
         <v>82</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{D5BD7720-F086-D143-B676-18BC52AE5F54}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{12BBD998-E940-674A-93A5-A8EF6FC0071E}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{0DE51B95-492B-9548-8275-9705C0A81065}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{8029C5AE-1B80-CF4F-A17B-EE35AF521196}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{4E7EADC2-EA50-3D4B-B9F2-4F2F43C94F42}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{E67CC30E-A8D9-2C43-BE7C-EA59FFAAA9F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1475,7 +1655,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1492,7 +1672,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1506,7 +1686,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1523,7 +1703,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1540,7 +1720,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -1557,7 +1737,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -1574,7 +1754,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1588,7 +1768,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -1605,7 +1785,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Better error message and improved test data
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B440BB-570F-BE43-A27A-4162B63B84B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E388142-9511-164B-81B0-2635746A56C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="3200" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="3200" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="116">
   <si>
     <t>Activity</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Fettes</t>
+  </si>
+  <si>
+    <t>Brot</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1630,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1745,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>113</v>
@@ -1748,10 +1754,10 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1761,28 +1767,28 @@
       <c r="B8" s="2" t="s">
         <v>113</v>
       </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1796,9 +1802,26 @@
         <v>104</v>
       </c>
       <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Append results of Testrun to existing file(s) + Updated examples
</commit_message>
<xml_diff>
--- a/examples/CompleteBaangtWebdemo.xlsx
+++ b/examples/CompleteBaangtWebdemo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E388142-9511-164B-81B0-2635746A56C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39299793-0BB6-F946-883D-4B4C30B72F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="3200" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63860" yWindow="7140" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="117">
   <si>
     <t>Activity</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Brot</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -1378,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1396,7 @@
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1418,8 +1421,11 @@
       <c r="H1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1441,8 +1447,11 @@
       <c r="G2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1461,8 +1470,11 @@
       <c r="G3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1484,8 +1496,11 @@
       <c r="G4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1507,8 +1522,11 @@
       <c r="G5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1527,8 +1545,11 @@
       <c r="G6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -1550,8 +1571,11 @@
       <c r="G7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1573,8 +1597,11 @@
       <c r="G8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -1593,8 +1620,11 @@
       <c r="G9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1615,6 +1645,9 @@
       </c>
       <c r="G10" t="s">
         <v>82</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1636,15 +1669,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1660,8 +1693,11 @@
       <c r="E1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1677,8 +1713,11 @@
       <c r="E2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1691,8 +1730,11 @@
       <c r="E3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1708,8 +1750,11 @@
       <c r="E4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1725,8 +1770,11 @@
       <c r="E5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -1742,8 +1790,11 @@
       <c r="E6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1759,8 +1810,11 @@
       <c r="E7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1776,8 +1830,11 @@
       <c r="E8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -1790,8 +1847,11 @@
       <c r="E9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -1807,8 +1867,11 @@
       <c r="E10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1823,6 +1886,9 @@
       </c>
       <c r="E11" t="s">
         <v>108</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>